<commit_message>
Add R2 and R3 Eagle files
</commit_message>
<xml_diff>
--- a/Moteino_BOM.xlsx
+++ b/Moteino_BOM.xlsx
@@ -96,9 +96,6 @@
     <t>Your favorite PCB fab</t>
   </si>
   <si>
-    <t>Sparkfun, ModernDevice, (hopefully LowPowerLab.com as well one day)</t>
-  </si>
-  <si>
     <t>MCP1700 3.3v (up to 6V in)</t>
   </si>
   <si>
@@ -118,6 +115,9 @@
   </si>
   <si>
     <t>?</t>
+  </si>
+  <si>
+    <t>lowpowerlab.com/shop</t>
   </si>
 </sst>
 </file>
@@ -536,7 +536,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D28" sqref="D28"/>
+      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -614,7 +614,7 @@
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C8" s="10">
         <v>1</v>
@@ -625,13 +625,13 @@
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="10">
+        <v>1</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>28</v>
-      </c>
-      <c r="C9" s="10">
-        <v>1</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
@@ -642,7 +642,7 @@
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
@@ -672,7 +672,7 @@
         <v>15</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>16</v>
@@ -680,13 +680,13 @@
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B14" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" s="4" t="s">
         <v>31</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
@@ -717,7 +717,7 @@
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C18" s="11"/>
     </row>

</xml_diff>